<commit_message>
Initial commit with leaderboard and Google Sheets integration
</commit_message>
<xml_diff>
--- a/reports/seeded_teams.xlsx
+++ b/reports/seeded_teams.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="600" firstSheet="0" activeTab="3" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Foosball" sheetId="1" state="visible" r:id="rId1"/>
@@ -864,6 +864,9 @@
           <t>w</t>
         </is>
       </c>
+      <c r="H10" t="n">
+        <v>7</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -897,6 +900,9 @@
           <t>w</t>
         </is>
       </c>
+      <c r="H11" t="n">
+        <v>7</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -925,6 +931,9 @@
       <c r="F12" t="n">
         <v>8</v>
       </c>
+      <c r="H12" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -953,6 +962,9 @@
       <c r="F13" t="n">
         <v>6</v>
       </c>
+      <c r="H13" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -981,6 +993,9 @@
       <c r="F14" t="n">
         <v>6</v>
       </c>
+      <c r="H14" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1075,6 +1090,9 @@
       <c r="F17" t="n">
         <v>4</v>
       </c>
+      <c r="H17" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1103,6 +1121,9 @@
       <c r="F18" t="n">
         <v>1</v>
       </c>
+      <c r="H18" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1131,6 +1152,9 @@
       <c r="F19" t="n">
         <v>8</v>
       </c>
+      <c r="H19" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1159,6 +1183,9 @@
       <c r="F20" t="n">
         <v>2</v>
       </c>
+      <c r="H20" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1187,6 +1214,9 @@
       <c r="F21" t="n">
         <v>3</v>
       </c>
+      <c r="H21" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1215,6 +1245,9 @@
       <c r="F22" t="n">
         <v>2</v>
       </c>
+      <c r="H22" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1243,6 +1276,9 @@
       <c r="F23" t="n">
         <v>4</v>
       </c>
+      <c r="H23" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -1271,6 +1307,9 @@
       <c r="F24" t="n">
         <v>3</v>
       </c>
+      <c r="H24" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -1298,6 +1337,9 @@
       </c>
       <c r="F25" t="n">
         <v>1</v>
+      </c>
+      <c r="H25" t="n">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -1687,6 +1729,9 @@
       <c r="F10" t="n">
         <v>3</v>
       </c>
+      <c r="H10" t="n">
+        <v>7</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1715,6 +1760,9 @@
       <c r="F11" t="n">
         <v>7</v>
       </c>
+      <c r="H11" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1743,6 +1791,9 @@
       <c r="F12" t="n">
         <v>1</v>
       </c>
+      <c r="H12" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1771,6 +1822,9 @@
       <c r="F13" t="n">
         <v>2</v>
       </c>
+      <c r="H13" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1799,6 +1853,9 @@
       <c r="F14" t="n">
         <v>2</v>
       </c>
+      <c r="H14" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1827,6 +1884,9 @@
       <c r="F15" t="n">
         <v>5</v>
       </c>
+      <c r="H15" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1855,6 +1915,9 @@
       <c r="F16" t="n">
         <v>4</v>
       </c>
+      <c r="H16" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1883,6 +1946,9 @@
       <c r="F17" t="n">
         <v>6</v>
       </c>
+      <c r="H17" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1911,6 +1977,9 @@
       <c r="F18" t="n">
         <v>3</v>
       </c>
+      <c r="H18" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1939,6 +2008,9 @@
       <c r="F19" t="n">
         <v>8</v>
       </c>
+      <c r="H19" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1967,6 +2039,9 @@
       <c r="F20" t="n">
         <v>6</v>
       </c>
+      <c r="H20" t="n">
+        <v>7</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1995,6 +2070,9 @@
       <c r="F21" t="n">
         <v>7</v>
       </c>
+      <c r="H21" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -2023,6 +2101,9 @@
       <c r="F22" t="n">
         <v>1</v>
       </c>
+      <c r="H22" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -2051,6 +2132,9 @@
       <c r="F23" t="n">
         <v>8</v>
       </c>
+      <c r="H23" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -2079,6 +2163,9 @@
       <c r="F24" t="n">
         <v>4</v>
       </c>
+      <c r="H24" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -2106,6 +2193,9 @@
       </c>
       <c r="F25" t="n">
         <v>5</v>
+      </c>
+      <c r="H25" t="n">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -2560,7 +2650,9 @@
         <v>2</v>
       </c>
       <c r="G10" t="inlineStr"/>
-      <c r="H10" t="inlineStr"/>
+      <c r="H10" t="n">
+        <v>3</v>
+      </c>
       <c r="I10" t="inlineStr"/>
       <c r="J10" t="inlineStr"/>
       <c r="K10" t="inlineStr"/>
@@ -2597,7 +2689,9 @@
         <v>1</v>
       </c>
       <c r="G11" t="inlineStr"/>
-      <c r="H11" t="inlineStr"/>
+      <c r="H11" t="n">
+        <v>1</v>
+      </c>
       <c r="I11" t="inlineStr"/>
       <c r="J11" t="inlineStr"/>
       <c r="K11" t="inlineStr"/>
@@ -2634,7 +2728,9 @@
         <v>3</v>
       </c>
       <c r="G12" t="inlineStr"/>
-      <c r="H12" t="inlineStr"/>
+      <c r="H12" t="n">
+        <v>8</v>
+      </c>
       <c r="I12" t="inlineStr"/>
       <c r="J12" t="inlineStr"/>
       <c r="K12" t="inlineStr"/>
@@ -2671,7 +2767,9 @@
         <v>5</v>
       </c>
       <c r="G13" t="inlineStr"/>
-      <c r="H13" t="inlineStr"/>
+      <c r="H13" t="n">
+        <v>5</v>
+      </c>
       <c r="I13" t="inlineStr"/>
       <c r="J13" t="inlineStr"/>
       <c r="K13" t="inlineStr"/>
@@ -2708,7 +2806,9 @@
         <v>3</v>
       </c>
       <c r="G14" t="inlineStr"/>
-      <c r="H14" t="inlineStr"/>
+      <c r="H14" t="n">
+        <v>4</v>
+      </c>
       <c r="I14" t="inlineStr"/>
       <c r="J14" t="inlineStr"/>
       <c r="K14" t="inlineStr"/>
@@ -2745,7 +2845,9 @@
         <v>2</v>
       </c>
       <c r="G15" t="inlineStr"/>
-      <c r="H15" t="inlineStr"/>
+      <c r="H15" t="n">
+        <v>7</v>
+      </c>
       <c r="I15" t="inlineStr"/>
       <c r="J15" t="inlineStr"/>
       <c r="K15" t="inlineStr"/>
@@ -2782,7 +2884,9 @@
         <v>7</v>
       </c>
       <c r="G16" t="inlineStr"/>
-      <c r="H16" t="inlineStr"/>
+      <c r="H16" t="n">
+        <v>1</v>
+      </c>
       <c r="I16" t="inlineStr"/>
       <c r="J16" t="inlineStr"/>
       <c r="K16" t="inlineStr"/>
@@ -2819,7 +2923,9 @@
         <v>6</v>
       </c>
       <c r="G17" t="inlineStr"/>
-      <c r="H17" t="inlineStr"/>
+      <c r="H17" t="n">
+        <v>6</v>
+      </c>
       <c r="I17" t="inlineStr"/>
       <c r="J17" t="inlineStr"/>
       <c r="K17" t="inlineStr"/>
@@ -2856,7 +2962,9 @@
         <v>4</v>
       </c>
       <c r="G18" t="inlineStr"/>
-      <c r="H18" t="inlineStr"/>
+      <c r="H18" t="n">
+        <v>2</v>
+      </c>
       <c r="I18" t="inlineStr"/>
       <c r="J18" t="inlineStr"/>
       <c r="K18" t="inlineStr"/>
@@ -2893,7 +3001,9 @@
         <v>1</v>
       </c>
       <c r="G19" t="inlineStr"/>
-      <c r="H19" t="inlineStr"/>
+      <c r="H19" t="n">
+        <v>6</v>
+      </c>
       <c r="I19" t="inlineStr"/>
       <c r="J19" t="inlineStr"/>
       <c r="K19" t="inlineStr"/>
@@ -2930,7 +3040,9 @@
         <v>7</v>
       </c>
       <c r="G20" t="inlineStr"/>
-      <c r="H20" t="inlineStr"/>
+      <c r="H20" t="n">
+        <v>4</v>
+      </c>
       <c r="I20" t="inlineStr"/>
       <c r="J20" t="inlineStr"/>
       <c r="K20" t="inlineStr"/>
@@ -2967,7 +3079,9 @@
         <v>8</v>
       </c>
       <c r="G21" t="inlineStr"/>
-      <c r="H21" t="inlineStr"/>
+      <c r="H21" t="n">
+        <v>5</v>
+      </c>
       <c r="I21" t="inlineStr"/>
       <c r="J21" t="inlineStr"/>
       <c r="K21" t="inlineStr"/>
@@ -3004,7 +3118,9 @@
         <v>5</v>
       </c>
       <c r="G22" t="inlineStr"/>
-      <c r="H22" t="inlineStr"/>
+      <c r="H22" t="n">
+        <v>3</v>
+      </c>
       <c r="I22" t="inlineStr"/>
       <c r="J22" t="inlineStr"/>
       <c r="K22" t="inlineStr"/>
@@ -3041,7 +3157,9 @@
         <v>4</v>
       </c>
       <c r="G23" t="inlineStr"/>
-      <c r="H23" t="inlineStr"/>
+      <c r="H23" t="n">
+        <v>2</v>
+      </c>
       <c r="I23" t="inlineStr"/>
       <c r="J23" t="inlineStr"/>
       <c r="K23" t="inlineStr"/>
@@ -3078,7 +3196,9 @@
         <v>6</v>
       </c>
       <c r="G24" t="inlineStr"/>
-      <c r="H24" t="inlineStr"/>
+      <c r="H24" t="n">
+        <v>8</v>
+      </c>
       <c r="I24" t="inlineStr"/>
       <c r="J24" t="inlineStr"/>
       <c r="K24" t="inlineStr"/>
@@ -3115,7 +3235,9 @@
         <v>8</v>
       </c>
       <c r="G25" t="inlineStr"/>
-      <c r="H25" t="inlineStr"/>
+      <c r="H25" t="n">
+        <v>7</v>
+      </c>
       <c r="I25" t="inlineStr"/>
       <c r="J25" t="inlineStr"/>
       <c r="K25" t="inlineStr"/>
@@ -3695,6 +3817,9 @@
       <c r="E18" t="n">
         <v>13</v>
       </c>
+      <c r="G18" t="n">
+        <v>15</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -3764,6 +3889,9 @@
       <c r="E21" t="n">
         <v>10</v>
       </c>
+      <c r="G21" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -3787,6 +3915,9 @@
       <c r="E22" t="n">
         <v>4</v>
       </c>
+      <c r="G22" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -3810,6 +3941,9 @@
       <c r="E23" t="n">
         <v>7</v>
       </c>
+      <c r="G23" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -3833,6 +3967,9 @@
       <c r="E24" t="n">
         <v>15</v>
       </c>
+      <c r="G24" t="n">
+        <v>13</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -3856,6 +3993,9 @@
       <c r="E25" t="n">
         <v>9</v>
       </c>
+      <c r="G25" t="n">
+        <v>7</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -3879,6 +4019,9 @@
       <c r="E26" t="n">
         <v>7</v>
       </c>
+      <c r="G26" t="n">
+        <v>13</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -3902,6 +4045,9 @@
       <c r="E27" t="n">
         <v>16</v>
       </c>
+      <c r="G27" t="n">
+        <v>11</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -3925,6 +4071,9 @@
       <c r="E28" t="n">
         <v>11</v>
       </c>
+      <c r="G28" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -3948,6 +4097,9 @@
       <c r="E29" t="n">
         <v>15</v>
       </c>
+      <c r="G29" t="n">
+        <v>14</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -3971,6 +4123,9 @@
       <c r="E30" t="n">
         <v>5</v>
       </c>
+      <c r="G30" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -3994,6 +4149,9 @@
       <c r="E31" t="n">
         <v>14</v>
       </c>
+      <c r="G31" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -4017,6 +4175,9 @@
       <c r="E32" t="n">
         <v>12</v>
       </c>
+      <c r="G32" t="n">
+        <v>12</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -4040,6 +4201,9 @@
       <c r="E33" t="n">
         <v>6</v>
       </c>
+      <c r="G33" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -4063,6 +4227,9 @@
       <c r="E34" t="n">
         <v>12</v>
       </c>
+      <c r="G34" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -4086,6 +4253,9 @@
       <c r="E35" t="n">
         <v>2</v>
       </c>
+      <c r="G35" t="n">
+        <v>12</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -4109,6 +4279,9 @@
       <c r="E36" t="n">
         <v>1</v>
       </c>
+      <c r="G36" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -4132,6 +4305,9 @@
       <c r="E37" t="n">
         <v>13</v>
       </c>
+      <c r="G37" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -4155,6 +4331,9 @@
       <c r="E38" t="n">
         <v>8</v>
       </c>
+      <c r="G38" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -4178,6 +4357,9 @@
       <c r="E39" t="n">
         <v>11</v>
       </c>
+      <c r="G39" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -4201,6 +4383,9 @@
       <c r="E40" t="n">
         <v>4</v>
       </c>
+      <c r="G40" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -4224,6 +4409,9 @@
       <c r="E41" t="n">
         <v>5</v>
       </c>
+      <c r="G41" t="n">
+        <v>14</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -4247,6 +4435,9 @@
       <c r="E42" t="n">
         <v>14</v>
       </c>
+      <c r="G42" t="n">
+        <v>11</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -4270,6 +4461,9 @@
       <c r="E43" t="n">
         <v>1</v>
       </c>
+      <c r="G43" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -4293,6 +4487,9 @@
       <c r="E44" t="n">
         <v>6</v>
       </c>
+      <c r="G44" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -4316,6 +4513,9 @@
       <c r="E45" t="n">
         <v>9</v>
       </c>
+      <c r="G45" t="n">
+        <v>7</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -4339,6 +4539,9 @@
       <c r="E46" t="n">
         <v>3</v>
       </c>
+      <c r="G46" t="n">
+        <v>15</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -4362,6 +4565,9 @@
       <c r="E47" t="n">
         <v>10</v>
       </c>
+      <c r="G47" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -4385,6 +4591,9 @@
       <c r="E48" t="n">
         <v>8</v>
       </c>
+      <c r="G48" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -4407,6 +4616,9 @@
       </c>
       <c r="E49" t="n">
         <v>2</v>
+      </c>
+      <c r="G49" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -4796,6 +5008,9 @@
       <c r="F10" t="n">
         <v>1</v>
       </c>
+      <c r="H10" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -4824,6 +5039,9 @@
       <c r="F11" t="n">
         <v>7</v>
       </c>
+      <c r="H11" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -4852,6 +5070,9 @@
       <c r="F12" t="n">
         <v>8</v>
       </c>
+      <c r="H12" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -4880,6 +5101,9 @@
       <c r="F13" t="n">
         <v>3</v>
       </c>
+      <c r="H13" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -4908,6 +5132,9 @@
       <c r="F14" t="n">
         <v>1</v>
       </c>
+      <c r="H14" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -4936,6 +5163,9 @@
       <c r="F15" t="n">
         <v>7</v>
       </c>
+      <c r="H15" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -4964,6 +5194,9 @@
       <c r="F16" t="n">
         <v>3</v>
       </c>
+      <c r="H16" t="n">
+        <v>7</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -4992,6 +5225,9 @@
       <c r="F17" t="n">
         <v>5</v>
       </c>
+      <c r="H17" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -5020,6 +5256,9 @@
       <c r="F18" t="n">
         <v>6</v>
       </c>
+      <c r="H18" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -5048,6 +5287,9 @@
       <c r="F19" t="n">
         <v>4</v>
       </c>
+      <c r="H19" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -5076,6 +5318,9 @@
       <c r="F20" t="n">
         <v>2</v>
       </c>
+      <c r="H20" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -5104,6 +5349,9 @@
       <c r="F21" t="n">
         <v>5</v>
       </c>
+      <c r="H21" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -5132,6 +5380,9 @@
       <c r="F22" t="n">
         <v>4</v>
       </c>
+      <c r="H22" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -5160,6 +5411,9 @@
       <c r="F23" t="n">
         <v>2</v>
       </c>
+      <c r="H23" t="n">
+        <v>7</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -5188,6 +5442,9 @@
       <c r="F24" t="n">
         <v>6</v>
       </c>
+      <c r="H24" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -5215,6 +5472,9 @@
       </c>
       <c r="F25" t="n">
         <v>8</v>
+      </c>
+      <c r="H25" t="n">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>